<commit_message>
Now loginToken is save to localStorage.
</commit_message>
<xml_diff>
--- a/meta/stores/AuthenticationControllerStore.xlsx
+++ b/meta/stores/AuthenticationControllerStore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/stores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236F9F7D-E53A-6F4F-AA99-9ED3078EE3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959B898D-876E-D248-B451-F518642D8EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="2040" windowWidth="26740" windowHeight="18960" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
   <si>
     <t>パッケージ</t>
   </si>
@@ -651,6 +651,14 @@
     <rPh sb="7" eb="9">
       <t xml:space="preserve">サンショウスル </t>
     </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>prepared</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>preparedFlg を true にします。</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1485,6 +1493,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1519,18 +1539,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1968,10 +1976,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K122"/>
+  <dimension ref="A1:K134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H130" sqref="H130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2268,10 +2276,10 @@
       <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A24" s="100" t="s">
+      <c r="A24" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="104" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="116" t="s">
@@ -2283,7 +2291,7 @@
       <c r="E24" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="106" t="s">
+      <c r="F24" s="110" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="116" t="s">
@@ -2295,12 +2303,12 @@
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="100"/>
-      <c r="B25" s="100"/>
+      <c r="A25" s="104"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="116"/>
       <c r="D25" s="116"/>
       <c r="E25" s="116"/>
-      <c r="F25" s="107"/>
+      <c r="F25" s="111"/>
       <c r="G25" s="116"/>
       <c r="H25" s="116"/>
       <c r="I25" s="18"/>
@@ -2583,20 +2591,20 @@
       <c r="K43" s="15"/>
     </row>
     <row r="44" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A44" s="100" t="s">
+      <c r="A44" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="100" t="s">
+      <c r="B44" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="101" t="s">
+      <c r="C44" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="102"/>
+      <c r="D44" s="106"/>
       <c r="E44" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="110"/>
+      <c r="F44" s="114"/>
       <c r="G44" s="116" t="s">
         <v>1</v>
       </c>
@@ -2606,12 +2614,12 @@
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="100"/>
-      <c r="B45" s="100"/>
-      <c r="C45" s="103"/>
-      <c r="D45" s="104"/>
+      <c r="A45" s="104"/>
+      <c r="B45" s="104"/>
+      <c r="C45" s="107"/>
+      <c r="D45" s="108"/>
       <c r="E45" s="116"/>
-      <c r="F45" s="111"/>
+      <c r="F45" s="115"/>
       <c r="G45" s="116"/>
       <c r="H45" s="116"/>
       <c r="I45" s="18"/>
@@ -2754,20 +2762,20 @@
       <c r="K56" s="15"/>
     </row>
     <row r="57" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A57" s="100" t="s">
+      <c r="A57" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="100" t="s">
+      <c r="B57" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="101" t="s">
+      <c r="C57" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="102"/>
+      <c r="D57" s="106"/>
       <c r="E57" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="F57" s="110"/>
+      <c r="F57" s="114"/>
       <c r="G57" s="116" t="s">
         <v>1</v>
       </c>
@@ -2777,12 +2785,12 @@
       <c r="K57" s="9"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="100"/>
-      <c r="B58" s="100"/>
-      <c r="C58" s="103"/>
-      <c r="D58" s="104"/>
+      <c r="A58" s="104"/>
+      <c r="B58" s="104"/>
+      <c r="C58" s="107"/>
+      <c r="D58" s="108"/>
       <c r="E58" s="116"/>
-      <c r="F58" s="111"/>
+      <c r="F58" s="115"/>
       <c r="G58" s="116"/>
       <c r="H58" s="116"/>
       <c r="I58" s="18"/>
@@ -3022,26 +3030,26 @@
       <c r="K76" s="15"/>
     </row>
     <row r="77" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A77" s="108" t="s">
+      <c r="A77" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="108" t="s">
+      <c r="B77" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="101" t="s">
+      <c r="C77" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="110"/>
-      <c r="E77" s="106" t="s">
+      <c r="D77" s="114"/>
+      <c r="E77" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="F77" s="106" t="s">
+      <c r="F77" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="G77" s="112" t="s">
+      <c r="G77" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="H77" s="114" t="s">
+      <c r="H77" s="102" t="s">
         <v>1</v>
       </c>
       <c r="I77" s="16"/>
@@ -3049,14 +3057,14 @@
       <c r="K77" s="9"/>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="109"/>
-      <c r="B78" s="109"/>
-      <c r="C78" s="103"/>
-      <c r="D78" s="111"/>
-      <c r="E78" s="107"/>
-      <c r="F78" s="107"/>
-      <c r="G78" s="113"/>
-      <c r="H78" s="115"/>
+      <c r="A78" s="113"/>
+      <c r="B78" s="113"/>
+      <c r="C78" s="107"/>
+      <c r="D78" s="115"/>
+      <c r="E78" s="111"/>
+      <c r="F78" s="111"/>
+      <c r="G78" s="101"/>
+      <c r="H78" s="103"/>
       <c r="I78" s="18"/>
       <c r="J78" s="29"/>
       <c r="K78" s="15"/>
@@ -3209,26 +3217,26 @@
       <c r="K89" s="15"/>
     </row>
     <row r="90" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A90" s="100" t="s">
+      <c r="A90" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="100" t="s">
+      <c r="B90" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="C90" s="101" t="s">
+      <c r="C90" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D90" s="102"/>
-      <c r="E90" s="105" t="s">
+      <c r="D90" s="106"/>
+      <c r="E90" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="F90" s="106" t="s">
+      <c r="F90" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="G90" s="112" t="s">
+      <c r="G90" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="H90" s="114" t="s">
+      <c r="H90" s="102" t="s">
         <v>1</v>
       </c>
       <c r="I90" s="16"/>
@@ -3236,14 +3244,14 @@
       <c r="K90" s="9"/>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="100"/>
-      <c r="B91" s="100"/>
-      <c r="C91" s="103"/>
-      <c r="D91" s="104"/>
-      <c r="E91" s="105"/>
-      <c r="F91" s="107"/>
-      <c r="G91" s="113"/>
-      <c r="H91" s="115"/>
+      <c r="A91" s="104"/>
+      <c r="B91" s="104"/>
+      <c r="C91" s="107"/>
+      <c r="D91" s="108"/>
+      <c r="E91" s="109"/>
+      <c r="F91" s="111"/>
+      <c r="G91" s="101"/>
+      <c r="H91" s="103"/>
       <c r="I91" s="18"/>
       <c r="J91" s="29"/>
       <c r="K91" s="15"/>
@@ -3392,26 +3400,26 @@
       <c r="K101" s="15"/>
     </row>
     <row r="102" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A102" s="100" t="s">
+      <c r="A102" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B102" s="100" t="s">
+      <c r="B102" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="C102" s="101" t="s">
+      <c r="C102" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D102" s="102"/>
-      <c r="E102" s="105" t="s">
+      <c r="D102" s="106"/>
+      <c r="E102" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="F102" s="106" t="s">
+      <c r="F102" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="G102" s="112" t="s">
+      <c r="G102" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="H102" s="114" t="s">
+      <c r="H102" s="102" t="s">
         <v>1</v>
       </c>
       <c r="I102" s="16"/>
@@ -3419,14 +3427,14 @@
       <c r="K102" s="9"/>
     </row>
     <row r="103" spans="1:11">
-      <c r="A103" s="100"/>
-      <c r="B103" s="100"/>
-      <c r="C103" s="103"/>
-      <c r="D103" s="104"/>
-      <c r="E103" s="105"/>
-      <c r="F103" s="107"/>
-      <c r="G103" s="113"/>
-      <c r="H103" s="115"/>
+      <c r="A103" s="104"/>
+      <c r="B103" s="104"/>
+      <c r="C103" s="107"/>
+      <c r="D103" s="108"/>
+      <c r="E103" s="109"/>
+      <c r="F103" s="111"/>
+      <c r="G103" s="101"/>
+      <c r="H103" s="103"/>
       <c r="I103" s="18"/>
       <c r="J103" s="29"/>
       <c r="K103" s="15"/>
@@ -3581,26 +3589,26 @@
       <c r="K113" s="15"/>
     </row>
     <row r="114" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A114" s="100" t="s">
+      <c r="A114" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B114" s="100" t="s">
+      <c r="B114" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="101" t="s">
+      <c r="C114" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D114" s="102"/>
-      <c r="E114" s="105" t="s">
+      <c r="D114" s="106"/>
+      <c r="E114" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="F114" s="106" t="s">
+      <c r="F114" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="G114" s="112" t="s">
+      <c r="G114" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="H114" s="114" t="s">
+      <c r="H114" s="102" t="s">
         <v>1</v>
       </c>
       <c r="I114" s="16"/>
@@ -3608,14 +3616,14 @@
       <c r="K114" s="9"/>
     </row>
     <row r="115" spans="1:11">
-      <c r="A115" s="100"/>
-      <c r="B115" s="100"/>
-      <c r="C115" s="103"/>
-      <c r="D115" s="104"/>
-      <c r="E115" s="105"/>
-      <c r="F115" s="107"/>
-      <c r="G115" s="113"/>
-      <c r="H115" s="115"/>
+      <c r="A115" s="104"/>
+      <c r="B115" s="104"/>
+      <c r="C115" s="107"/>
+      <c r="D115" s="108"/>
+      <c r="E115" s="109"/>
+      <c r="F115" s="111"/>
+      <c r="G115" s="101"/>
+      <c r="H115" s="103"/>
       <c r="I115" s="18"/>
       <c r="J115" s="29"/>
       <c r="K115" s="15"/>
@@ -3736,8 +3744,189 @@
       <c r="J122" s="27"/>
       <c r="K122" s="15"/>
     </row>
+    <row r="124" spans="1:11">
+      <c r="A124" s="13"/>
+      <c r="B124" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C124" s="13"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
+      <c r="F124" s="13"/>
+      <c r="G124" s="13"/>
+      <c r="H124" s="13"/>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B125" s="14"/>
+      <c r="C125" s="14"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="14"/>
+      <c r="I125" s="14"/>
+      <c r="J125" s="6"/>
+      <c r="K125" s="15"/>
+    </row>
+    <row r="126" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A126" s="104" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" s="104" t="s">
+        <v>3</v>
+      </c>
+      <c r="C126" s="105" t="s">
+        <v>4</v>
+      </c>
+      <c r="D126" s="106"/>
+      <c r="E126" s="109" t="s">
+        <v>6</v>
+      </c>
+      <c r="F126" s="110" t="s">
+        <v>47</v>
+      </c>
+      <c r="G126" s="100" t="s">
+        <v>39</v>
+      </c>
+      <c r="H126" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="I126" s="16"/>
+      <c r="J126" s="17"/>
+      <c r="K126" s="9"/>
+    </row>
+    <row r="127" spans="1:11">
+      <c r="A127" s="104"/>
+      <c r="B127" s="104"/>
+      <c r="C127" s="107"/>
+      <c r="D127" s="108"/>
+      <c r="E127" s="109"/>
+      <c r="F127" s="111"/>
+      <c r="G127" s="101"/>
+      <c r="H127" s="103"/>
+      <c r="I127" s="18"/>
+      <c r="J127" s="29"/>
+      <c r="K127" s="15"/>
+    </row>
+    <row r="128" spans="1:11">
+      <c r="A128" s="19">
+        <v>1</v>
+      </c>
+      <c r="B128" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="C128" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="D128" s="88"/>
+      <c r="E128" s="82"/>
+      <c r="F128" s="68"/>
+      <c r="G128" s="91"/>
+      <c r="H128" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="I128" s="21"/>
+      <c r="J128" s="28"/>
+      <c r="K128" s="15"/>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="A129" s="19">
+        <f>A128+1</f>
+        <v>2</v>
+      </c>
+      <c r="B129" s="70"/>
+      <c r="C129" s="85"/>
+      <c r="D129" s="88"/>
+      <c r="E129" s="82"/>
+      <c r="F129" s="68"/>
+      <c r="G129" s="91"/>
+      <c r="H129" s="20"/>
+      <c r="I129" s="21"/>
+      <c r="J129" s="28"/>
+      <c r="K129" s="15"/>
+    </row>
+    <row r="130" spans="1:11">
+      <c r="A130" s="19">
+        <f t="shared" ref="A130:A133" si="7">A129+1</f>
+        <v>3</v>
+      </c>
+      <c r="B130" s="71"/>
+      <c r="C130" s="86"/>
+      <c r="D130" s="88"/>
+      <c r="E130" s="88"/>
+      <c r="F130" s="68"/>
+      <c r="G130" s="91"/>
+      <c r="H130" s="93"/>
+      <c r="I130" s="21"/>
+      <c r="J130" s="22"/>
+      <c r="K130" s="15"/>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="A131" s="19">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B131" s="72"/>
+      <c r="C131" s="87"/>
+      <c r="D131" s="88"/>
+      <c r="E131" s="82"/>
+      <c r="F131" s="68"/>
+      <c r="G131" s="91"/>
+      <c r="H131" s="93"/>
+      <c r="I131" s="21"/>
+      <c r="J131" s="22"/>
+      <c r="K131" s="15"/>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="19">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="B132" s="72"/>
+      <c r="C132" s="87"/>
+      <c r="D132" s="88"/>
+      <c r="E132" s="82"/>
+      <c r="F132" s="68"/>
+      <c r="G132" s="91"/>
+      <c r="H132" s="93"/>
+      <c r="I132" s="21"/>
+      <c r="J132" s="22"/>
+      <c r="K132" s="15"/>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="A133" s="19">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B133" s="72"/>
+      <c r="C133" s="87"/>
+      <c r="D133" s="89"/>
+      <c r="E133" s="83"/>
+      <c r="F133" s="74"/>
+      <c r="G133" s="94"/>
+      <c r="H133" s="95"/>
+      <c r="I133" s="75"/>
+      <c r="J133" s="76"/>
+      <c r="K133" s="15"/>
+    </row>
+    <row r="134" spans="1:11">
+      <c r="A134" s="23"/>
+      <c r="B134" s="24"/>
+      <c r="C134" s="25"/>
+      <c r="D134" s="90"/>
+      <c r="E134" s="84"/>
+      <c r="F134" s="69"/>
+      <c r="G134" s="97"/>
+      <c r="H134" s="98"/>
+      <c r="I134" s="26"/>
+      <c r="J134" s="27"/>
+      <c r="K134" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="58">
     <mergeCell ref="G102:G103"/>
     <mergeCell ref="H102:H103"/>
     <mergeCell ref="A114:A115"/>
@@ -3789,6 +3978,13 @@
     <mergeCell ref="C90:D91"/>
     <mergeCell ref="E90:E91"/>
     <mergeCell ref="F90:F91"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="H126:H127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="C126:D127"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="3">
@@ -3798,7 +3994,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:F32 F92:G98 F79:G85 F104:G110 F116:G122" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:F32 F92:G98 F79:G85 F104:G110 F116:G122 F128:G134" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Correct authentication status. TODO: Do same action to pageTransitData Status.
</commit_message>
<xml_diff>
--- a/meta/stores/AuthenticationControllerStore.xlsx
+++ b/meta/stores/AuthenticationControllerStore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/stores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE5944D-A79D-A646-88EC-07011567F6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FB5EB3-49A7-5042-BD2E-6B9F84B68F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="2040" windowWidth="26740" windowHeight="18960" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
   <si>
     <t>パッケージ</t>
   </si>
@@ -469,10 +469,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>boolean</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>AuthenticationControllerStore</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -528,20 +524,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>toggleすることで loginInfo を LocalStorage から store にロードします。</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>toggleすることでtore 上の loginInfo を LocalStorage に保管します。</t>
-    <rPh sb="16" eb="17">
-      <t xml:space="preserve">ジョウノ </t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t xml:space="preserve">ホカンシマス。 </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>update</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -567,42 +549,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>loginInfo が有効である事を示します。</t>
-    <rPh sb="11" eb="13">
-      <t xml:space="preserve">ユウコウ </t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t xml:space="preserve">シメシマス。 </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>saveFlg</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>restoreFlg</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>preparedFlg</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>removeFlg</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>loginInfor LocalStorage から削除し、store には空の LoginInfo をセットします。</t>
-    <rPh sb="26" eb="28">
-      <t xml:space="preserve">サクジョ </t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t xml:space="preserve">ノ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>remove</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -654,11 +600,66 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>prepared</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>preparedFlg を true にします。</t>
+    <t>status</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"invalid"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ログイン状態です。&lt;br&gt;
+* valid : ログインが完了している状態です。&lt;br&gt;
+* invlid : 未ログイン状態です。&lt;br&gt;
+* restoring : localStorageに保管されたログイン情報をロード中です&lt;br&gt;
+* saving : ログイン情報をlocalStorageに保管中です&lt;br&gt;
+* removing : localStorage からログイン情報を削除します&lt;br&gt;</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ログインジョウタイ </t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t xml:space="preserve">カンリョウ </t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t xml:space="preserve">ジョウタイ </t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t xml:space="preserve">ミ </t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t xml:space="preserve">ジョウタイ </t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t xml:space="preserve">ホカンサレタ </t>
+    </rPh>
+    <rPh sb="144" eb="147">
+      <t xml:space="preserve">ホカンチュウ </t>
+    </rPh>
+    <rPh sb="185" eb="187">
+      <t xml:space="preserve">サクジョ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>setStatus</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>statusの値を変更します。</t>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">アタイヲ </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">ヘンコウシマｓ。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ログイン状態</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1326,7 +1327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1529,6 +1530,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1553,16 +1566,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1978,8 +2009,8 @@
   </sheetPr>
   <dimension ref="A1:K134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129:J129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2028,7 +2059,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
@@ -2043,7 +2074,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="33"/>
       <c r="E7" s="11"/>
@@ -2053,10 +2084,10 @@
       <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="113" t="s">
+      <c r="A8" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="114"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
@@ -2068,10 +2099,10 @@
       <c r="G8" s="35"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="113" t="s">
+      <c r="A9" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="114"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="81" t="s">
         <v>29</v>
       </c>
@@ -2087,11 +2118,11 @@
         <v>1</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="115" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="116"/>
-      <c r="E10" s="117"/>
+      <c r="C10" s="119" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="120"/>
+      <c r="E10" s="121"/>
       <c r="F10" s="65"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -2126,10 +2157,10 @@
       <c r="G12"/>
     </row>
     <row r="13" spans="1:11" s="32" customFormat="1">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="119"/>
+      <c r="B13" s="123"/>
       <c r="C13" s="64" t="s">
         <v>14</v>
       </c>
@@ -2190,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
@@ -2282,22 +2313,22 @@
       <c r="B24" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="112" t="s">
+      <c r="C24" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="112" t="s">
+      <c r="D24" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="112" t="s">
+      <c r="E24" s="116" t="s">
         <v>5</v>
       </c>
       <c r="F24" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="112" t="s">
+      <c r="G24" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="112"/>
+      <c r="H24" s="116"/>
       <c r="I24" s="16"/>
       <c r="J24" s="17"/>
       <c r="K24" s="9"/>
@@ -2305,12 +2336,12 @@
     <row r="25" spans="1:11">
       <c r="A25" s="104"/>
       <c r="B25" s="104"/>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="112"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
       <c r="F25" s="111"/>
-      <c r="G25" s="112"/>
-      <c r="H25" s="112"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="116"/>
       <c r="I25" s="18"/>
       <c r="J25" s="29"/>
       <c r="K25" s="15"/>
@@ -2320,46 +2351,46 @@
         <v>1</v>
       </c>
       <c r="B26" s="70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="28"/>
       <c r="K26" s="15"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" ht="94" customHeight="1">
       <c r="A27" s="19">
         <f>A26+1</f>
         <v>2</v>
       </c>
-      <c r="B27" s="70" t="s">
-        <v>69</v>
+      <c r="B27" s="77" t="s">
+        <v>74</v>
       </c>
       <c r="C27" s="77" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="28"/>
+        <v>75</v>
+      </c>
+      <c r="D27" s="127"/>
+      <c r="E27" s="127" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="127"/>
+      <c r="G27" s="124" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="125"/>
+      <c r="I27" s="125"/>
+      <c r="J27" s="126"/>
       <c r="K27" s="15"/>
     </row>
     <row r="28" spans="1:11">
@@ -2367,19 +2398,19 @@
         <f t="shared" ref="A28:A30" si="0">A27+1</f>
         <v>3</v>
       </c>
-      <c r="B28" s="71" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="77" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20" t="s">
-        <v>62</v>
+      <c r="B28" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73" t="s">
+        <v>73</v>
       </c>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
@@ -2391,20 +2422,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B29" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="78" t="s">
-        <v>51</v>
-      </c>
+      <c r="B29" s="72"/>
+      <c r="C29" s="78"/>
       <c r="D29" s="20"/>
-      <c r="E29" s="20" t="b">
-        <v>0</v>
-      </c>
+      <c r="E29" s="20"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="20" t="s">
-        <v>68</v>
-      </c>
+      <c r="G29" s="20"/>
       <c r="H29" s="21"/>
       <c r="I29" s="21"/>
       <c r="J29" s="22"/>
@@ -2415,20 +2438,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B30" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="78" t="s">
-        <v>51</v>
-      </c>
+      <c r="B30" s="72"/>
+      <c r="C30" s="78"/>
       <c r="D30" s="20"/>
-      <c r="E30" s="20" t="b">
-        <v>0</v>
-      </c>
+      <c r="E30" s="20"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="20" t="s">
-        <v>73</v>
-      </c>
+      <c r="G30" s="20"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
       <c r="J30" s="22"/>
@@ -2438,20 +2453,12 @@
       <c r="A31" s="19">
         <v>6</v>
       </c>
-      <c r="B31" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="78" t="s">
-        <v>78</v>
-      </c>
+      <c r="B31" s="72"/>
+      <c r="C31" s="78"/>
       <c r="D31" s="73"/>
-      <c r="E31" s="73" t="s">
-        <v>81</v>
-      </c>
+      <c r="E31" s="73"/>
       <c r="F31" s="73"/>
-      <c r="G31" s="73" t="s">
-        <v>82</v>
-      </c>
+      <c r="G31" s="73"/>
       <c r="H31" s="75"/>
       <c r="I31" s="75"/>
       <c r="J31" s="76"/>
@@ -2601,14 +2608,14 @@
         <v>4</v>
       </c>
       <c r="D44" s="106"/>
-      <c r="E44" s="112" t="s">
+      <c r="E44" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="120"/>
-      <c r="G44" s="112" t="s">
+      <c r="F44" s="114"/>
+      <c r="G44" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="112"/>
+      <c r="H44" s="116"/>
       <c r="I44" s="16"/>
       <c r="J44" s="17"/>
       <c r="K44" s="9"/>
@@ -2618,10 +2625,10 @@
       <c r="B45" s="104"/>
       <c r="C45" s="107"/>
       <c r="D45" s="108"/>
-      <c r="E45" s="112"/>
-      <c r="F45" s="121"/>
-      <c r="G45" s="112"/>
-      <c r="H45" s="112"/>
+      <c r="E45" s="116"/>
+      <c r="F45" s="115"/>
+      <c r="G45" s="116"/>
+      <c r="H45" s="116"/>
       <c r="I45" s="18"/>
       <c r="J45" s="29"/>
       <c r="K45" s="15"/>
@@ -2772,14 +2779,14 @@
         <v>4</v>
       </c>
       <c r="D57" s="106"/>
-      <c r="E57" s="112" t="s">
+      <c r="E57" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="F57" s="120"/>
-      <c r="G57" s="112" t="s">
+      <c r="F57" s="114"/>
+      <c r="G57" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="H57" s="112"/>
+      <c r="H57" s="116"/>
       <c r="I57" s="16"/>
       <c r="J57" s="17"/>
       <c r="K57" s="9"/>
@@ -2789,10 +2796,10 @@
       <c r="B58" s="104"/>
       <c r="C58" s="107"/>
       <c r="D58" s="108"/>
-      <c r="E58" s="112"/>
-      <c r="F58" s="121"/>
-      <c r="G58" s="112"/>
-      <c r="H58" s="112"/>
+      <c r="E58" s="116"/>
+      <c r="F58" s="115"/>
+      <c r="G58" s="116"/>
+      <c r="H58" s="116"/>
       <c r="I58" s="18"/>
       <c r="J58" s="29"/>
       <c r="K58" s="15"/>
@@ -2944,7 +2951,7 @@
         <v>1</v>
       </c>
       <c r="B70" s="46" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C70" s="38"/>
       <c r="D70" s="38"/>
@@ -3030,16 +3037,16 @@
       <c r="K76" s="15"/>
     </row>
     <row r="77" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A77" s="122" t="s">
+      <c r="A77" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="122" t="s">
+      <c r="B77" s="112" t="s">
         <v>3</v>
       </c>
       <c r="C77" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="120"/>
+      <c r="D77" s="114"/>
       <c r="E77" s="110" t="s">
         <v>6</v>
       </c>
@@ -3057,10 +3064,10 @@
       <c r="K77" s="9"/>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="123"/>
-      <c r="B78" s="123"/>
+      <c r="A78" s="113"/>
+      <c r="B78" s="113"/>
       <c r="C78" s="107"/>
-      <c r="D78" s="121"/>
+      <c r="D78" s="115"/>
       <c r="E78" s="111"/>
       <c r="F78" s="111"/>
       <c r="G78" s="101"/>
@@ -3074,7 +3081,7 @@
         <v>1</v>
       </c>
       <c r="B79" s="70" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C79" s="85" t="s">
         <v>46</v>
@@ -3084,7 +3091,7 @@
       <c r="F79" s="68"/>
       <c r="G79" s="91"/>
       <c r="H79" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I79" s="92"/>
       <c r="J79" s="28"/>
@@ -3096,17 +3103,17 @@
         <v>2</v>
       </c>
       <c r="B80" s="70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C80" s="85" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D80" s="88"/>
       <c r="E80" s="82"/>
       <c r="F80" s="68"/>
       <c r="G80" s="91"/>
       <c r="H80" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I80" s="92"/>
       <c r="J80" s="28"/>
@@ -3261,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="B92" s="70" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C92" s="85" t="s">
         <v>46</v>
@@ -3273,7 +3280,7 @@
       </c>
       <c r="G92" s="91"/>
       <c r="H92" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I92" s="21"/>
       <c r="J92" s="28"/>
@@ -3444,7 +3451,7 @@
         <v>1</v>
       </c>
       <c r="B104" s="70" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C104" s="85" t="s">
         <v>46</v>
@@ -3456,7 +3463,7 @@
       </c>
       <c r="G104" s="91"/>
       <c r="H104" s="20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I104" s="21"/>
       <c r="J104" s="28"/>
@@ -3468,17 +3475,17 @@
         <v>2</v>
       </c>
       <c r="B105" s="70" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C105" s="85" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D105" s="88"/>
       <c r="E105" s="82"/>
       <c r="F105" s="68"/>
       <c r="G105" s="91"/>
       <c r="H105" s="20" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="I105" s="21"/>
       <c r="J105" s="28"/>
@@ -3633,7 +3640,7 @@
         <v>1</v>
       </c>
       <c r="B116" s="70" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C116" s="85" t="s">
         <v>46</v>
@@ -3645,7 +3652,7 @@
       </c>
       <c r="G116" s="91"/>
       <c r="H116" s="20" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I116" s="21"/>
       <c r="J116" s="28"/>
@@ -3816,7 +3823,7 @@
         <v>1</v>
       </c>
       <c r="B128" s="70" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C128" s="85" t="s">
         <v>46</v>
@@ -3826,26 +3833,32 @@
       <c r="F128" s="68"/>
       <c r="G128" s="91"/>
       <c r="H128" s="20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I128" s="21"/>
       <c r="J128" s="28"/>
       <c r="K128" s="15"/>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" ht="84" customHeight="1">
       <c r="A129" s="19">
         <f>A128+1</f>
         <v>2</v>
       </c>
-      <c r="B129" s="70"/>
-      <c r="C129" s="85"/>
-      <c r="D129" s="88"/>
-      <c r="E129" s="82"/>
-      <c r="F129" s="68"/>
-      <c r="G129" s="91"/>
-      <c r="H129" s="20"/>
-      <c r="I129" s="21"/>
-      <c r="J129" s="28"/>
+      <c r="B129" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="C129" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="D129" s="131"/>
+      <c r="E129" s="132"/>
+      <c r="F129" s="133"/>
+      <c r="G129" s="127"/>
+      <c r="H129" s="128" t="s">
+        <v>80</v>
+      </c>
+      <c r="I129" s="129"/>
+      <c r="J129" s="130"/>
       <c r="K129" s="15"/>
     </row>
     <row r="130" spans="1:11">
@@ -3926,51 +3939,9 @@
       <c r="K134" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="H126:H127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="C126:D127"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:D91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="G90:G91"/>
-    <mergeCell ref="H90:H91"/>
-    <mergeCell ref="C44:D45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:H45"/>
-    <mergeCell ref="G57:H58"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G24:H25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="A13:B13"/>
+  <mergeCells count="60">
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="H129:J129"/>
     <mergeCell ref="G102:G103"/>
     <mergeCell ref="H102:H103"/>
     <mergeCell ref="A114:A115"/>
@@ -3985,6 +3956,50 @@
     <mergeCell ref="C102:D103"/>
     <mergeCell ref="E102:E103"/>
     <mergeCell ref="F102:F103"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="G24:H25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="G90:G91"/>
+    <mergeCell ref="H90:H91"/>
+    <mergeCell ref="C44:D45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:H45"/>
+    <mergeCell ref="G57:H58"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="H126:H127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="C126:D127"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="3">
@@ -3994,7 +4009,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:F32 F92:G98 F79:G85 F104:G110 F116:G122 F128:G134" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F128:G134 F92:G98 F79:G85 F104:G110 F116:G122 F26:F32" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Logout sample is implemented. * to remove authStore and pageTransitDataStore on logout. * try to load pageTransiData on page load.
</commit_message>
<xml_diff>
--- a/meta/stores/AuthenticationControllerStore.xlsx
+++ b/meta/stores/AuthenticationControllerStore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/stores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFE36A7-B3C4-C343-A54D-A700A2D5B401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ABEFA1-BB67-1B49-9C02-058A06AD8768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="2040" windowWidth="26740" windowHeight="18960" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="87">
   <si>
     <t>パッケージ</t>
   </si>
@@ -689,6 +689,48 @@
     </rPh>
     <rPh sb="320" eb="322">
       <t xml:space="preserve">セイコウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>issuer</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>restore, saveなどの更新操作を行ったコンポーネントのId</t>
+    <rPh sb="16" eb="20">
+      <t xml:space="preserve">コウシンソウサ </t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t xml:space="preserve">オコナッタ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"default"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>更新を発行したコンポーネントです</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">コウシン </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">ハッコウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>setIssuer</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>issuerの値を変更します。</t>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">アタイヲ </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">ヘンコウシマｓ。 </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1536,6 +1578,78 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1553,78 +1667,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2037,10 +2079,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K134"/>
+  <dimension ref="A1:K148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H142" sqref="H142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2114,10 +2156,10 @@
       <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="123" t="s">
+      <c r="A8" s="121" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="124"/>
+      <c r="B8" s="122"/>
       <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
@@ -2129,10 +2171,10 @@
       <c r="G8" s="35"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="123" t="s">
+      <c r="A9" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="124"/>
+      <c r="B9" s="122"/>
       <c r="C9" s="81" t="s">
         <v>29</v>
       </c>
@@ -2148,11 +2190,11 @@
         <v>1</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="125" t="s">
+      <c r="C10" s="123" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="126"/>
-      <c r="E10" s="127"/>
+      <c r="D10" s="124"/>
+      <c r="E10" s="125"/>
       <c r="F10" s="65"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -2187,10 +2229,10 @@
       <c r="G12"/>
     </row>
     <row r="13" spans="1:11" s="32" customFormat="1">
-      <c r="A13" s="128" t="s">
+      <c r="A13" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="129"/>
+      <c r="B13" s="127"/>
       <c r="C13" s="64" t="s">
         <v>14</v>
       </c>
@@ -2337,41 +2379,41 @@
       <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A24" s="114" t="s">
+      <c r="A24" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="114" t="s">
+      <c r="B24" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="122" t="s">
+      <c r="C24" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="122" t="s">
+      <c r="D24" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="122" t="s">
+      <c r="E24" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="120" t="s">
+      <c r="F24" s="114" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="122" t="s">
+      <c r="G24" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="122"/>
+      <c r="H24" s="120"/>
       <c r="I24" s="16"/>
       <c r="J24" s="17"/>
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="114"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="122"/>
-      <c r="D25" s="122"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="121"/>
-      <c r="G25" s="122"/>
-      <c r="H25" s="122"/>
+      <c r="A25" s="108"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="120"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="120"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="120"/>
+      <c r="H25" s="120"/>
       <c r="I25" s="18"/>
       <c r="J25" s="29"/>
       <c r="K25" s="15"/>
@@ -2399,7 +2441,7 @@
       <c r="J26" s="28"/>
       <c r="K26" s="15"/>
     </row>
-    <row r="27" spans="1:11" ht="94" customHeight="1">
+    <row r="27" spans="1:11" ht="164" customHeight="1">
       <c r="A27" s="19">
         <f>A26+1</f>
         <v>2</v>
@@ -2415,17 +2457,17 @@
         <v>76</v>
       </c>
       <c r="F27" s="100"/>
-      <c r="G27" s="104" t="s">
+      <c r="G27" s="128" t="s">
         <v>80</v>
       </c>
-      <c r="H27" s="105"/>
-      <c r="I27" s="105"/>
-      <c r="J27" s="106"/>
+      <c r="H27" s="129"/>
+      <c r="I27" s="129"/>
+      <c r="J27" s="130"/>
       <c r="K27" s="15"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="19">
-        <f t="shared" ref="A28:A30" si="0">A27+1</f>
+        <f t="shared" ref="A28:A31" si="0">A27+1</f>
         <v>3</v>
       </c>
       <c r="B28" s="72" t="s">
@@ -2452,12 +2494,20 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B29" s="72"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
+      <c r="B29" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="73"/>
+      <c r="E29" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="73"/>
+      <c r="G29" s="73" t="s">
+        <v>82</v>
+      </c>
       <c r="H29" s="21"/>
       <c r="I29" s="21"/>
       <c r="J29" s="22"/>
@@ -2465,8 +2515,8 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="19">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>A28+1</f>
+        <v>4</v>
       </c>
       <c r="B30" s="72"/>
       <c r="C30" s="78"/>
@@ -2481,85 +2531,88 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="19">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="B31" s="72"/>
       <c r="C31" s="78"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="76"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="22"/>
       <c r="K31" s="15"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="27"/>
+      <c r="A32" s="19">
+        <v>6</v>
+      </c>
+      <c r="B32" s="72"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="76"/>
       <c r="K32" s="15"/>
     </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="30" t="s">
+    <row r="33" spans="1:11">
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="15"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="44" t="s">
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="47" t="s">
+      <c r="G36" s="44"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B37" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="80"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="35"/>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="51"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
       <c r="K37" s="35"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="51"/>
       <c r="B38" s="46"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="67"/>
       <c r="G38" s="34"/>
       <c r="H38" s="36"/>
@@ -2568,11 +2621,11 @@
       <c r="K38" s="35"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="52"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="50"/>
+      <c r="A39" s="51"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41"/>
       <c r="F39" s="67"/>
       <c r="G39" s="34"/>
       <c r="H39" s="36"/>
@@ -2581,14 +2634,17 @@
       <c r="K39" s="35"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="35"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="13"/>
@@ -2602,9 +2658,7 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="13"/>
-      <c r="B42" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
@@ -2613,75 +2667,71 @@
       <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="15"/>
-    </row>
-    <row r="44" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A44" s="114" t="s">
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="15"/>
+    </row>
+    <row r="45" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A45" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="114" t="s">
+      <c r="B45" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="115" t="s">
+      <c r="C45" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="116"/>
-      <c r="E44" s="122" t="s">
+      <c r="D45" s="110"/>
+      <c r="E45" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="130"/>
-      <c r="G44" s="122" t="s">
+      <c r="F45" s="118"/>
+      <c r="G45" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="122"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="9"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="114"/>
-      <c r="B45" s="114"/>
-      <c r="C45" s="117"/>
-      <c r="D45" s="118"/>
-      <c r="E45" s="122"/>
-      <c r="F45" s="131"/>
-      <c r="G45" s="122"/>
-      <c r="H45" s="122"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="15"/>
+      <c r="H45" s="120"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="9"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="19">
-        <v>1</v>
-      </c>
-      <c r="B46" s="70"/>
-      <c r="C46" s="85"/>
-      <c r="D46" s="88"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="28"/>
+      <c r="A46" s="108"/>
+      <c r="B46" s="108"/>
+      <c r="C46" s="111"/>
+      <c r="D46" s="112"/>
+      <c r="E46" s="120"/>
+      <c r="F46" s="119"/>
+      <c r="G46" s="120"/>
+      <c r="H46" s="120"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="29"/>
       <c r="K46" s="15"/>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="19">
-        <f>A46+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B47" s="70"/>
       <c r="C47" s="85"/>
@@ -2696,27 +2746,27 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="19">
-        <f t="shared" ref="A48:A51" si="1">A47+1</f>
-        <v>3</v>
-      </c>
-      <c r="B48" s="71"/>
-      <c r="C48" s="86"/>
+        <f>A47+1</f>
+        <v>2</v>
+      </c>
+      <c r="B48" s="70"/>
+      <c r="C48" s="85"/>
       <c r="D48" s="88"/>
       <c r="E48" s="20"/>
       <c r="F48" s="82"/>
       <c r="G48" s="20"/>
       <c r="H48" s="21"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="22"/>
+      <c r="J48" s="28"/>
       <c r="K48" s="15"/>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="19">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B49" s="72"/>
-      <c r="C49" s="87"/>
+        <f t="shared" ref="A49:A52" si="1">A48+1</f>
+        <v>3</v>
+      </c>
+      <c r="B49" s="71"/>
+      <c r="C49" s="86"/>
       <c r="D49" s="88"/>
       <c r="E49" s="20"/>
       <c r="F49" s="82"/>
@@ -2729,7 +2779,7 @@
     <row r="50" spans="1:11">
       <c r="A50" s="19">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B50" s="72"/>
       <c r="C50" s="87"/>
@@ -2745,114 +2795,114 @@
     <row r="51" spans="1:11">
       <c r="A51" s="19">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B51" s="72"/>
       <c r="C51" s="87"/>
-      <c r="D51" s="89"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="83"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="75"/>
-      <c r="I51" s="75"/>
-      <c r="J51" s="76"/>
+      <c r="D51" s="88"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="82"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="22"/>
       <c r="K51" s="15"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="23"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="84"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="27"/>
+      <c r="A52" s="19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B52" s="72"/>
+      <c r="C52" s="87"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="75"/>
+      <c r="I52" s="75"/>
+      <c r="J52" s="76"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13" t="s">
+    <row r="53" spans="1:11">
+      <c r="A53" s="23"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="90"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="84"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="15"/>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="13"/>
+      <c r="B56" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="3" t="s">
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="15"/>
-    </row>
-    <row r="57" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A57" s="114" t="s">
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="15"/>
+    </row>
+    <row r="58" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A58" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="114" t="s">
+      <c r="B58" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="115" t="s">
+      <c r="C58" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="116"/>
-      <c r="E57" s="122" t="s">
+      <c r="D58" s="110"/>
+      <c r="E58" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="F57" s="130"/>
-      <c r="G57" s="122" t="s">
+      <c r="F58" s="118"/>
+      <c r="G58" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="H57" s="122"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="17"/>
-      <c r="K57" s="9"/>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="114"/>
-      <c r="B58" s="114"/>
-      <c r="C58" s="117"/>
-      <c r="D58" s="118"/>
-      <c r="E58" s="122"/>
-      <c r="F58" s="131"/>
-      <c r="G58" s="122"/>
-      <c r="H58" s="122"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="15"/>
+      <c r="H58" s="120"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="9"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="19">
-        <v>1</v>
-      </c>
-      <c r="B59" s="70"/>
-      <c r="C59" s="85"/>
-      <c r="D59" s="88"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="82"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="28"/>
+      <c r="A59" s="108"/>
+      <c r="B59" s="108"/>
+      <c r="C59" s="111"/>
+      <c r="D59" s="112"/>
+      <c r="E59" s="120"/>
+      <c r="F59" s="119"/>
+      <c r="G59" s="120"/>
+      <c r="H59" s="120"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="29"/>
       <c r="K59" s="15"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="19">
-        <f>A59+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B60" s="70"/>
       <c r="C60" s="85"/>
@@ -2867,27 +2917,27 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="19">
-        <f t="shared" ref="A61:A64" si="2">A60+1</f>
-        <v>3</v>
-      </c>
-      <c r="B61" s="71"/>
-      <c r="C61" s="86"/>
+        <f>A60+1</f>
+        <v>2</v>
+      </c>
+      <c r="B61" s="70"/>
+      <c r="C61" s="85"/>
       <c r="D61" s="88"/>
       <c r="E61" s="20"/>
       <c r="F61" s="82"/>
       <c r="G61" s="20"/>
       <c r="H61" s="21"/>
       <c r="I61" s="21"/>
-      <c r="J61" s="22"/>
+      <c r="J61" s="28"/>
       <c r="K61" s="15"/>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="19">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="B62" s="72"/>
-      <c r="C62" s="87"/>
+        <f t="shared" ref="A62:A65" si="2">A61+1</f>
+        <v>3</v>
+      </c>
+      <c r="B62" s="71"/>
+      <c r="C62" s="86"/>
       <c r="D62" s="88"/>
       <c r="E62" s="20"/>
       <c r="F62" s="82"/>
@@ -2900,7 +2950,7 @@
     <row r="63" spans="1:11">
       <c r="A63" s="19">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B63" s="72"/>
       <c r="C63" s="87"/>
@@ -2916,89 +2966,92 @@
     <row r="64" spans="1:11">
       <c r="A64" s="19">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B64" s="72"/>
       <c r="C64" s="87"/>
-      <c r="D64" s="89"/>
-      <c r="E64" s="73"/>
-      <c r="F64" s="83"/>
-      <c r="G64" s="73"/>
-      <c r="H64" s="75"/>
-      <c r="I64" s="75"/>
-      <c r="J64" s="76"/>
+      <c r="D64" s="88"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="82"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="22"/>
       <c r="K64" s="15"/>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="23"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="90"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="84"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="26"/>
-      <c r="I65" s="26"/>
-      <c r="J65" s="27"/>
+      <c r="A65" s="19">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B65" s="72"/>
+      <c r="C65" s="87"/>
+      <c r="D65" s="89"/>
+      <c r="E65" s="73"/>
+      <c r="F65" s="83"/>
+      <c r="G65" s="73"/>
+      <c r="H65" s="75"/>
+      <c r="I65" s="75"/>
+      <c r="J65" s="76"/>
       <c r="K65" s="15"/>
     </row>
-    <row r="68" spans="1:11">
-      <c r="A68" s="30" t="s">
+    <row r="66" spans="1:11">
+      <c r="A66" s="23"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="90"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="84"/>
+      <c r="G66" s="25"/>
+      <c r="H66" s="26"/>
+      <c r="I66" s="26"/>
+      <c r="J66" s="27"/>
+      <c r="K66" s="15"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="79"/>
-      <c r="F68" s="44" t="s">
+      <c r="B69" s="31"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="79"/>
+      <c r="F69" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="G68" s="44"/>
-      <c r="H68" s="43"/>
-      <c r="I68" s="43"/>
-      <c r="J68" s="43"/>
-      <c r="K68" s="43"/>
-    </row>
-    <row r="69" spans="1:11">
-      <c r="A69" s="47" t="s">
+      <c r="G69" s="44"/>
+      <c r="H69" s="43"/>
+      <c r="I69" s="43"/>
+      <c r="J69" s="43"/>
+      <c r="K69" s="43"/>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B69" s="42" t="s">
+      <c r="B70" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C69" s="42"/>
-      <c r="D69" s="42"/>
-      <c r="E69" s="80"/>
-      <c r="F69" s="66"/>
-      <c r="G69" s="66"/>
-      <c r="H69" s="44"/>
-      <c r="I69" s="45"/>
-      <c r="J69" s="45"/>
-      <c r="K69" s="35"/>
-    </row>
-    <row r="70" spans="1:11">
-      <c r="A70" s="51">
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="80"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
+      <c r="H70" s="44"/>
+      <c r="I70" s="45"/>
+      <c r="J70" s="45"/>
+      <c r="K70" s="35"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="51">
         <v>1</v>
       </c>
-      <c r="B70" s="46" t="s">
+      <c r="B71" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="38"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="67"/>
-      <c r="G70" s="34"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="36"/>
-      <c r="J70" s="36"/>
-      <c r="K70" s="35"/>
-    </row>
-    <row r="71" spans="1:11">
-      <c r="A71" s="51"/>
-      <c r="B71" s="46"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40"/>
-      <c r="E71" s="41"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="39"/>
       <c r="F71" s="67"/>
       <c r="G71" s="34"/>
       <c r="H71" s="36"/>
@@ -3007,11 +3060,11 @@
       <c r="K71" s="35"/>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="52"/>
-      <c r="B72" s="48"/>
-      <c r="C72" s="49"/>
-      <c r="D72" s="49"/>
-      <c r="E72" s="50"/>
+      <c r="A72" s="51"/>
+      <c r="B72" s="46"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="41"/>
       <c r="F72" s="67"/>
       <c r="G72" s="34"/>
       <c r="H72" s="36"/>
@@ -3020,14 +3073,17 @@
       <c r="K72" s="35"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="13"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
+      <c r="A73" s="52"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="49"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="67"/>
+      <c r="G73" s="34"/>
+      <c r="H73" s="36"/>
+      <c r="I73" s="36"/>
+      <c r="J73" s="36"/>
+      <c r="K73" s="35"/>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="13"/>
@@ -3041,9 +3097,7 @@
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="13"/>
-      <c r="B75" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
@@ -3052,98 +3106,88 @@
       <c r="H75" s="13"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="13"/>
+      <c r="B76" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="15"/>
-    </row>
-    <row r="77" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A77" s="132" t="s">
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="15"/>
+    </row>
+    <row r="78" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A78" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="132" t="s">
+      <c r="B78" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="115" t="s">
+      <c r="C78" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="130"/>
-      <c r="E77" s="120" t="s">
+      <c r="D78" s="118"/>
+      <c r="E78" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="F77" s="120" t="s">
+      <c r="F78" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="G77" s="110" t="s">
+      <c r="G78" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="H77" s="112" t="s">
+      <c r="H78" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="I77" s="16"/>
-      <c r="J77" s="17"/>
-      <c r="K77" s="9"/>
-    </row>
-    <row r="78" spans="1:11">
-      <c r="A78" s="133"/>
-      <c r="B78" s="133"/>
-      <c r="C78" s="117"/>
-      <c r="D78" s="131"/>
-      <c r="E78" s="121"/>
-      <c r="F78" s="121"/>
-      <c r="G78" s="111"/>
-      <c r="H78" s="113"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="29"/>
-      <c r="K78" s="15"/>
+      <c r="I78" s="16"/>
+      <c r="J78" s="17"/>
+      <c r="K78" s="9"/>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="19">
-        <v>1</v>
-      </c>
-      <c r="B79" s="70" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" s="85" t="s">
-        <v>46</v>
-      </c>
-      <c r="D79" s="88"/>
-      <c r="E79" s="82"/>
-      <c r="F79" s="68"/>
-      <c r="G79" s="91"/>
-      <c r="H79" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I79" s="92"/>
-      <c r="J79" s="28"/>
+      <c r="A79" s="117"/>
+      <c r="B79" s="117"/>
+      <c r="C79" s="111"/>
+      <c r="D79" s="119"/>
+      <c r="E79" s="115"/>
+      <c r="F79" s="115"/>
+      <c r="G79" s="105"/>
+      <c r="H79" s="107"/>
+      <c r="I79" s="18"/>
+      <c r="J79" s="29"/>
       <c r="K79" s="15"/>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="19">
-        <f>A79+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B80" s="70" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C80" s="85" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D80" s="88"/>
       <c r="E80" s="82"/>
       <c r="F80" s="68"/>
       <c r="G80" s="91"/>
       <c r="H80" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I80" s="92"/>
       <c r="J80" s="28"/>
@@ -3151,32 +3195,44 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="19">
-        <f t="shared" ref="A81:A84" si="3">A80+1</f>
-        <v>3</v>
-      </c>
-      <c r="B81" s="71"/>
-      <c r="C81" s="86"/>
+        <f>A80+1</f>
+        <v>2</v>
+      </c>
+      <c r="B81" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="C81" s="85" t="s">
+        <v>54</v>
+      </c>
       <c r="D81" s="88"/>
-      <c r="E81" s="88"/>
+      <c r="E81" s="82"/>
       <c r="F81" s="68"/>
       <c r="G81" s="91"/>
-      <c r="H81" s="93"/>
+      <c r="H81" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="I81" s="92"/>
-      <c r="J81" s="22"/>
+      <c r="J81" s="28"/>
       <c r="K81" s="15"/>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="19">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="B82" s="72"/>
-      <c r="C82" s="87"/>
+        <f t="shared" ref="A82:A85" si="3">A81+1</f>
+        <v>3</v>
+      </c>
+      <c r="B82" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" s="86" t="s">
+        <v>75</v>
+      </c>
       <c r="D82" s="88"/>
-      <c r="E82" s="82"/>
+      <c r="E82" s="88"/>
       <c r="F82" s="68"/>
       <c r="G82" s="91"/>
-      <c r="H82" s="93"/>
+      <c r="H82" s="93" t="s">
+        <v>84</v>
+      </c>
       <c r="I82" s="92"/>
       <c r="J82" s="22"/>
       <c r="K82" s="15"/>
@@ -3184,7 +3240,7 @@
     <row r="83" spans="1:11">
       <c r="A83" s="19">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B83" s="72"/>
       <c r="C83" s="87"/>
@@ -3200,163 +3256,169 @@
     <row r="84" spans="1:11">
       <c r="A84" s="19">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B84" s="72"/>
       <c r="C84" s="87"/>
-      <c r="D84" s="89"/>
-      <c r="E84" s="83"/>
-      <c r="F84" s="74"/>
-      <c r="G84" s="94"/>
-      <c r="H84" s="95"/>
-      <c r="I84" s="96"/>
-      <c r="J84" s="76"/>
+      <c r="D84" s="88"/>
+      <c r="E84" s="82"/>
+      <c r="F84" s="68"/>
+      <c r="G84" s="91"/>
+      <c r="H84" s="93"/>
+      <c r="I84" s="92"/>
+      <c r="J84" s="22"/>
       <c r="K84" s="15"/>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="23"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="90"/>
-      <c r="E85" s="84"/>
-      <c r="F85" s="69"/>
-      <c r="G85" s="97"/>
-      <c r="H85" s="98"/>
-      <c r="I85" s="99"/>
-      <c r="J85" s="27"/>
+      <c r="A85" s="19">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="B85" s="72"/>
+      <c r="C85" s="87"/>
+      <c r="D85" s="89"/>
+      <c r="E85" s="83"/>
+      <c r="F85" s="74"/>
+      <c r="G85" s="94"/>
+      <c r="H85" s="95"/>
+      <c r="I85" s="96"/>
+      <c r="J85" s="76"/>
       <c r="K85" s="15"/>
     </row>
-    <row r="88" spans="1:11">
-      <c r="A88" s="13"/>
-      <c r="B88" s="13" t="s">
+    <row r="86" spans="1:11">
+      <c r="A86" s="23"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="90"/>
+      <c r="E86" s="84"/>
+      <c r="F86" s="69"/>
+      <c r="G86" s="97"/>
+      <c r="H86" s="98"/>
+      <c r="I86" s="99"/>
+      <c r="J86" s="27"/>
+      <c r="K86" s="15"/>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89" s="13"/>
+      <c r="B89" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-    </row>
-    <row r="89" spans="1:11">
-      <c r="A89" s="3" t="s">
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="6"/>
-      <c r="K89" s="15"/>
-    </row>
-    <row r="90" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A90" s="114" t="s">
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="15"/>
+    </row>
+    <row r="91" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A91" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="114" t="s">
+      <c r="B91" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C90" s="115" t="s">
+      <c r="C91" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="D90" s="116"/>
-      <c r="E90" s="119" t="s">
+      <c r="D91" s="110"/>
+      <c r="E91" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="F90" s="120" t="s">
+      <c r="F91" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="G90" s="110" t="s">
+      <c r="G91" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="H90" s="112" t="s">
+      <c r="H91" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="I90" s="16"/>
-      <c r="J90" s="17"/>
-      <c r="K90" s="9"/>
-    </row>
-    <row r="91" spans="1:11">
-      <c r="A91" s="114"/>
-      <c r="B91" s="114"/>
-      <c r="C91" s="117"/>
-      <c r="D91" s="118"/>
-      <c r="E91" s="119"/>
-      <c r="F91" s="121"/>
-      <c r="G91" s="111"/>
-      <c r="H91" s="113"/>
-      <c r="I91" s="18"/>
-      <c r="J91" s="29"/>
-      <c r="K91" s="15"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="17"/>
+      <c r="K91" s="9"/>
     </row>
     <row r="92" spans="1:11">
-      <c r="A92" s="19">
-        <v>1</v>
-      </c>
-      <c r="B92" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="C92" s="85" t="s">
-        <v>46</v>
-      </c>
-      <c r="D92" s="88"/>
-      <c r="E92" s="82"/>
-      <c r="F92" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="G92" s="91"/>
-      <c r="H92" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="I92" s="21"/>
-      <c r="J92" s="28"/>
+      <c r="A92" s="108"/>
+      <c r="B92" s="108"/>
+      <c r="C92" s="111"/>
+      <c r="D92" s="112"/>
+      <c r="E92" s="113"/>
+      <c r="F92" s="115"/>
+      <c r="G92" s="105"/>
+      <c r="H92" s="107"/>
+      <c r="I92" s="18"/>
+      <c r="J92" s="29"/>
       <c r="K92" s="15"/>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" s="19">
-        <f>A92+1</f>
-        <v>2</v>
-      </c>
-      <c r="B93" s="70"/>
-      <c r="C93" s="85"/>
+        <v>1</v>
+      </c>
+      <c r="B93" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C93" s="85" t="s">
+        <v>46</v>
+      </c>
       <c r="D93" s="88"/>
       <c r="E93" s="82"/>
-      <c r="F93" s="68"/>
+      <c r="F93" s="68" t="s">
+        <v>14</v>
+      </c>
       <c r="G93" s="91"/>
-      <c r="H93" s="20"/>
+      <c r="H93" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="I93" s="21"/>
       <c r="J93" s="28"/>
       <c r="K93" s="15"/>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="19">
-        <f t="shared" ref="A94:A97" si="4">A93+1</f>
-        <v>3</v>
-      </c>
-      <c r="B94" s="71"/>
-      <c r="C94" s="86"/>
+        <f>A93+1</f>
+        <v>2</v>
+      </c>
+      <c r="B94" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C94" s="85" t="s">
+        <v>75</v>
+      </c>
       <c r="D94" s="88"/>
-      <c r="E94" s="88"/>
+      <c r="E94" s="82"/>
       <c r="F94" s="68"/>
       <c r="G94" s="91"/>
-      <c r="H94" s="93"/>
+      <c r="H94" s="93" t="s">
+        <v>84</v>
+      </c>
       <c r="I94" s="21"/>
-      <c r="J94" s="22"/>
+      <c r="J94" s="28"/>
       <c r="K94" s="15"/>
     </row>
     <row r="95" spans="1:11">
       <c r="A95" s="19">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="B95" s="72"/>
-      <c r="C95" s="87"/>
+        <f t="shared" ref="A95:A98" si="4">A94+1</f>
+        <v>3</v>
+      </c>
+      <c r="B95" s="71"/>
+      <c r="C95" s="86"/>
       <c r="D95" s="88"/>
-      <c r="E95" s="82"/>
+      <c r="E95" s="88"/>
       <c r="F95" s="68"/>
       <c r="G95" s="91"/>
       <c r="H95" s="93"/>
@@ -3367,7 +3429,7 @@
     <row r="96" spans="1:11">
       <c r="A96" s="19">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B96" s="72"/>
       <c r="C96" s="87"/>
@@ -3383,139 +3445,133 @@
     <row r="97" spans="1:11">
       <c r="A97" s="19">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B97" s="72"/>
       <c r="C97" s="87"/>
-      <c r="D97" s="89"/>
-      <c r="E97" s="83"/>
-      <c r="F97" s="74"/>
-      <c r="G97" s="94"/>
-      <c r="H97" s="95"/>
-      <c r="I97" s="75"/>
-      <c r="J97" s="76"/>
+      <c r="D97" s="88"/>
+      <c r="E97" s="82"/>
+      <c r="F97" s="68"/>
+      <c r="G97" s="91"/>
+      <c r="H97" s="93"/>
+      <c r="I97" s="21"/>
+      <c r="J97" s="22"/>
       <c r="K97" s="15"/>
     </row>
     <row r="98" spans="1:11">
-      <c r="A98" s="23"/>
-      <c r="B98" s="24"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="90"/>
-      <c r="E98" s="84"/>
-      <c r="F98" s="69"/>
-      <c r="G98" s="97"/>
-      <c r="H98" s="98"/>
-      <c r="I98" s="26"/>
-      <c r="J98" s="27"/>
+      <c r="A98" s="19">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="B98" s="72"/>
+      <c r="C98" s="87"/>
+      <c r="D98" s="89"/>
+      <c r="E98" s="83"/>
+      <c r="F98" s="74"/>
+      <c r="G98" s="94"/>
+      <c r="H98" s="95"/>
+      <c r="I98" s="75"/>
+      <c r="J98" s="76"/>
       <c r="K98" s="15"/>
     </row>
-    <row r="100" spans="1:11">
-      <c r="A100" s="13"/>
-      <c r="B100" s="13" t="s">
+    <row r="99" spans="1:11">
+      <c r="A99" s="23"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="25"/>
+      <c r="D99" s="90"/>
+      <c r="E99" s="84"/>
+      <c r="F99" s="69"/>
+      <c r="G99" s="97"/>
+      <c r="H99" s="98"/>
+      <c r="I99" s="26"/>
+      <c r="J99" s="27"/>
+      <c r="K99" s="15"/>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" s="13"/>
+      <c r="B101" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
-    </row>
-    <row r="101" spans="1:11">
-      <c r="A101" s="3" t="s">
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B101" s="14"/>
-      <c r="C101" s="14"/>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14"/>
-      <c r="G101" s="14"/>
-      <c r="H101" s="14"/>
-      <c r="I101" s="14"/>
-      <c r="J101" s="6"/>
-      <c r="K101" s="15"/>
-    </row>
-    <row r="102" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A102" s="114" t="s">
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="15"/>
+    </row>
+    <row r="103" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A103" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="B102" s="114" t="s">
+      <c r="B103" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C102" s="115" t="s">
+      <c r="C103" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="D102" s="116"/>
-      <c r="E102" s="119" t="s">
+      <c r="D103" s="110"/>
+      <c r="E103" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="F102" s="120" t="s">
+      <c r="F103" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="G102" s="110" t="s">
+      <c r="G103" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="H102" s="112" t="s">
+      <c r="H103" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="I102" s="16"/>
-      <c r="J102" s="17"/>
-      <c r="K102" s="9"/>
-    </row>
-    <row r="103" spans="1:11">
-      <c r="A103" s="114"/>
-      <c r="B103" s="114"/>
-      <c r="C103" s="117"/>
-      <c r="D103" s="118"/>
-      <c r="E103" s="119"/>
-      <c r="F103" s="121"/>
-      <c r="G103" s="111"/>
-      <c r="H103" s="113"/>
-      <c r="I103" s="18"/>
-      <c r="J103" s="29"/>
-      <c r="K103" s="15"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="17"/>
+      <c r="K103" s="9"/>
     </row>
     <row r="104" spans="1:11">
-      <c r="A104" s="19">
-        <v>1</v>
-      </c>
-      <c r="B104" s="70" t="s">
-        <v>57</v>
-      </c>
-      <c r="C104" s="85" t="s">
-        <v>46</v>
-      </c>
-      <c r="D104" s="88"/>
-      <c r="E104" s="82"/>
-      <c r="F104" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="G104" s="91"/>
-      <c r="H104" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I104" s="21"/>
-      <c r="J104" s="28"/>
+      <c r="A104" s="108"/>
+      <c r="B104" s="108"/>
+      <c r="C104" s="111"/>
+      <c r="D104" s="112"/>
+      <c r="E104" s="113"/>
+      <c r="F104" s="115"/>
+      <c r="G104" s="105"/>
+      <c r="H104" s="107"/>
+      <c r="I104" s="18"/>
+      <c r="J104" s="29"/>
       <c r="K104" s="15"/>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="19">
-        <f>A104+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B105" s="70" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C105" s="85" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D105" s="88"/>
       <c r="E105" s="82"/>
-      <c r="F105" s="68"/>
+      <c r="F105" s="68" t="s">
+        <v>14</v>
+      </c>
       <c r="G105" s="91"/>
       <c r="H105" s="20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I105" s="21"/>
       <c r="J105" s="28"/>
@@ -3523,32 +3579,44 @@
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="19">
-        <f t="shared" ref="A106:A109" si="5">A105+1</f>
-        <v>3</v>
-      </c>
-      <c r="B106" s="71"/>
-      <c r="C106" s="86"/>
+        <f>A105+1</f>
+        <v>2</v>
+      </c>
+      <c r="B106" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="C106" s="85" t="s">
+        <v>69</v>
+      </c>
       <c r="D106" s="88"/>
-      <c r="E106" s="88"/>
+      <c r="E106" s="82"/>
       <c r="F106" s="68"/>
       <c r="G106" s="91"/>
-      <c r="H106" s="93"/>
+      <c r="H106" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="I106" s="21"/>
-      <c r="J106" s="22"/>
+      <c r="J106" s="28"/>
       <c r="K106" s="15"/>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="19">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="B107" s="72"/>
-      <c r="C107" s="87"/>
+        <f t="shared" ref="A107:A110" si="5">A106+1</f>
+        <v>3</v>
+      </c>
+      <c r="B107" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C107" s="85" t="s">
+        <v>75</v>
+      </c>
       <c r="D107" s="88"/>
       <c r="E107" s="82"/>
       <c r="F107" s="68"/>
       <c r="G107" s="91"/>
-      <c r="H107" s="93"/>
+      <c r="H107" s="93" t="s">
+        <v>84</v>
+      </c>
       <c r="I107" s="21"/>
       <c r="J107" s="22"/>
       <c r="K107" s="15"/>
@@ -3556,7 +3624,7 @@
     <row r="108" spans="1:11">
       <c r="A108" s="19">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B108" s="72"/>
       <c r="C108" s="87"/>
@@ -3572,163 +3640,169 @@
     <row r="109" spans="1:11">
       <c r="A109" s="19">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B109" s="72"/>
       <c r="C109" s="87"/>
-      <c r="D109" s="89"/>
-      <c r="E109" s="83"/>
-      <c r="F109" s="74"/>
-      <c r="G109" s="94"/>
-      <c r="H109" s="95"/>
-      <c r="I109" s="75"/>
-      <c r="J109" s="76"/>
+      <c r="D109" s="88"/>
+      <c r="E109" s="82"/>
+      <c r="F109" s="68"/>
+      <c r="G109" s="91"/>
+      <c r="H109" s="93"/>
+      <c r="I109" s="21"/>
+      <c r="J109" s="22"/>
       <c r="K109" s="15"/>
     </row>
     <row r="110" spans="1:11">
-      <c r="A110" s="23"/>
-      <c r="B110" s="24"/>
-      <c r="C110" s="25"/>
-      <c r="D110" s="90"/>
-      <c r="E110" s="84"/>
-      <c r="F110" s="69"/>
-      <c r="G110" s="97"/>
-      <c r="H110" s="98"/>
-      <c r="I110" s="26"/>
-      <c r="J110" s="27"/>
+      <c r="A110" s="19">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B110" s="72"/>
+      <c r="C110" s="87"/>
+      <c r="D110" s="89"/>
+      <c r="E110" s="83"/>
+      <c r="F110" s="74"/>
+      <c r="G110" s="94"/>
+      <c r="H110" s="95"/>
+      <c r="I110" s="75"/>
+      <c r="J110" s="76"/>
       <c r="K110" s="15"/>
     </row>
-    <row r="112" spans="1:11">
-      <c r="A112" s="13"/>
-      <c r="B112" s="13" t="s">
+    <row r="111" spans="1:11">
+      <c r="A111" s="23"/>
+      <c r="B111" s="24"/>
+      <c r="C111" s="25"/>
+      <c r="D111" s="90"/>
+      <c r="E111" s="84"/>
+      <c r="F111" s="69"/>
+      <c r="G111" s="97"/>
+      <c r="H111" s="98"/>
+      <c r="I111" s="26"/>
+      <c r="J111" s="27"/>
+      <c r="K111" s="15"/>
+    </row>
+    <row r="113" spans="1:11">
+      <c r="A113" s="13"/>
+      <c r="B113" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C112" s="13"/>
-      <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
-      <c r="G112" s="13"/>
-      <c r="H112" s="13"/>
-    </row>
-    <row r="113" spans="1:11">
-      <c r="A113" s="3" t="s">
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
+    </row>
+    <row r="114" spans="1:11">
+      <c r="A114" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B113" s="14"/>
-      <c r="C113" s="14"/>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14"/>
-      <c r="G113" s="14"/>
-      <c r="H113" s="14"/>
-      <c r="I113" s="14"/>
-      <c r="J113" s="6"/>
-      <c r="K113" s="15"/>
-    </row>
-    <row r="114" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A114" s="114" t="s">
+      <c r="B114" s="14"/>
+      <c r="C114" s="14"/>
+      <c r="D114" s="14"/>
+      <c r="E114" s="14"/>
+      <c r="F114" s="14"/>
+      <c r="G114" s="14"/>
+      <c r="H114" s="14"/>
+      <c r="I114" s="14"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="15"/>
+    </row>
+    <row r="115" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A115" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="B114" s="114" t="s">
+      <c r="B115" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="115" t="s">
+      <c r="C115" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="D114" s="116"/>
-      <c r="E114" s="119" t="s">
+      <c r="D115" s="110"/>
+      <c r="E115" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="F114" s="120" t="s">
+      <c r="F115" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="G114" s="110" t="s">
+      <c r="G115" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="H114" s="112" t="s">
+      <c r="H115" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="I114" s="16"/>
-      <c r="J114" s="17"/>
-      <c r="K114" s="9"/>
-    </row>
-    <row r="115" spans="1:11">
-      <c r="A115" s="114"/>
-      <c r="B115" s="114"/>
-      <c r="C115" s="117"/>
-      <c r="D115" s="118"/>
-      <c r="E115" s="119"/>
-      <c r="F115" s="121"/>
-      <c r="G115" s="111"/>
-      <c r="H115" s="113"/>
-      <c r="I115" s="18"/>
-      <c r="J115" s="29"/>
-      <c r="K115" s="15"/>
+      <c r="I115" s="16"/>
+      <c r="J115" s="17"/>
+      <c r="K115" s="9"/>
     </row>
     <row r="116" spans="1:11">
-      <c r="A116" s="19">
-        <v>1</v>
-      </c>
-      <c r="B116" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="C116" s="85" t="s">
-        <v>46</v>
-      </c>
-      <c r="D116" s="88"/>
-      <c r="E116" s="82"/>
-      <c r="F116" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="G116" s="91"/>
-      <c r="H116" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I116" s="21"/>
-      <c r="J116" s="28"/>
+      <c r="A116" s="108"/>
+      <c r="B116" s="108"/>
+      <c r="C116" s="111"/>
+      <c r="D116" s="112"/>
+      <c r="E116" s="113"/>
+      <c r="F116" s="115"/>
+      <c r="G116" s="105"/>
+      <c r="H116" s="107"/>
+      <c r="I116" s="18"/>
+      <c r="J116" s="29"/>
       <c r="K116" s="15"/>
     </row>
     <row r="117" spans="1:11">
       <c r="A117" s="19">
-        <f>A116+1</f>
-        <v>2</v>
-      </c>
-      <c r="B117" s="70"/>
-      <c r="C117" s="85"/>
+        <v>1</v>
+      </c>
+      <c r="B117" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="C117" s="85" t="s">
+        <v>46</v>
+      </c>
       <c r="D117" s="88"/>
       <c r="E117" s="82"/>
-      <c r="F117" s="68"/>
+      <c r="F117" s="68" t="s">
+        <v>14</v>
+      </c>
       <c r="G117" s="91"/>
-      <c r="H117" s="20"/>
+      <c r="H117" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="I117" s="21"/>
       <c r="J117" s="28"/>
       <c r="K117" s="15"/>
     </row>
     <row r="118" spans="1:11">
       <c r="A118" s="19">
-        <f t="shared" ref="A118:A121" si="6">A117+1</f>
-        <v>3</v>
-      </c>
-      <c r="B118" s="71"/>
-      <c r="C118" s="86"/>
+        <f>A117+1</f>
+        <v>2</v>
+      </c>
+      <c r="B118" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C118" s="85" t="s">
+        <v>75</v>
+      </c>
       <c r="D118" s="88"/>
-      <c r="E118" s="88"/>
+      <c r="E118" s="82"/>
       <c r="F118" s="68"/>
       <c r="G118" s="91"/>
-      <c r="H118" s="93"/>
+      <c r="H118" s="93" t="s">
+        <v>84</v>
+      </c>
       <c r="I118" s="21"/>
-      <c r="J118" s="22"/>
+      <c r="J118" s="28"/>
       <c r="K118" s="15"/>
     </row>
     <row r="119" spans="1:11">
       <c r="A119" s="19">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="B119" s="72"/>
-      <c r="C119" s="87"/>
+        <f t="shared" ref="A119:A122" si="6">A118+1</f>
+        <v>3</v>
+      </c>
+      <c r="B119" s="71"/>
+      <c r="C119" s="86"/>
       <c r="D119" s="88"/>
-      <c r="E119" s="82"/>
+      <c r="E119" s="88"/>
       <c r="F119" s="68"/>
       <c r="G119" s="91"/>
       <c r="H119" s="93"/>
@@ -3739,7 +3813,7 @@
     <row r="120" spans="1:11">
       <c r="A120" s="19">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B120" s="72"/>
       <c r="C120" s="87"/>
@@ -3755,170 +3829,176 @@
     <row r="121" spans="1:11">
       <c r="A121" s="19">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B121" s="72"/>
       <c r="C121" s="87"/>
-      <c r="D121" s="89"/>
-      <c r="E121" s="83"/>
-      <c r="F121" s="74"/>
-      <c r="G121" s="94"/>
-      <c r="H121" s="95"/>
-      <c r="I121" s="75"/>
-      <c r="J121" s="76"/>
+      <c r="D121" s="88"/>
+      <c r="E121" s="82"/>
+      <c r="F121" s="68"/>
+      <c r="G121" s="91"/>
+      <c r="H121" s="93"/>
+      <c r="I121" s="21"/>
+      <c r="J121" s="22"/>
       <c r="K121" s="15"/>
     </row>
     <row r="122" spans="1:11">
-      <c r="A122" s="23"/>
-      <c r="B122" s="24"/>
-      <c r="C122" s="25"/>
-      <c r="D122" s="90"/>
-      <c r="E122" s="84"/>
-      <c r="F122" s="69"/>
-      <c r="G122" s="97"/>
-      <c r="H122" s="98"/>
-      <c r="I122" s="26"/>
-      <c r="J122" s="27"/>
+      <c r="A122" s="19">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="B122" s="72"/>
+      <c r="C122" s="87"/>
+      <c r="D122" s="89"/>
+      <c r="E122" s="83"/>
+      <c r="F122" s="74"/>
+      <c r="G122" s="94"/>
+      <c r="H122" s="95"/>
+      <c r="I122" s="75"/>
+      <c r="J122" s="76"/>
       <c r="K122" s="15"/>
     </row>
-    <row r="124" spans="1:11">
-      <c r="A124" s="13"/>
-      <c r="B124" s="13" t="s">
+    <row r="123" spans="1:11">
+      <c r="A123" s="23"/>
+      <c r="B123" s="24"/>
+      <c r="C123" s="25"/>
+      <c r="D123" s="90"/>
+      <c r="E123" s="84"/>
+      <c r="F123" s="69"/>
+      <c r="G123" s="97"/>
+      <c r="H123" s="98"/>
+      <c r="I123" s="26"/>
+      <c r="J123" s="27"/>
+      <c r="K123" s="15"/>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" s="13"/>
+      <c r="B125" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C124" s="13"/>
-      <c r="D124" s="13"/>
-      <c r="E124" s="13"/>
-      <c r="F124" s="13"/>
-      <c r="G124" s="13"/>
-      <c r="H124" s="13"/>
-    </row>
-    <row r="125" spans="1:11">
-      <c r="A125" s="3" t="s">
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="13"/>
+      <c r="G125" s="13"/>
+      <c r="H125" s="13"/>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="A126" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B125" s="14"/>
-      <c r="C125" s="14"/>
-      <c r="D125" s="14"/>
-      <c r="E125" s="14"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="14"/>
-      <c r="H125" s="14"/>
-      <c r="I125" s="14"/>
-      <c r="J125" s="6"/>
-      <c r="K125" s="15"/>
-    </row>
-    <row r="126" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A126" s="114" t="s">
+      <c r="B126" s="14"/>
+      <c r="C126" s="14"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+      <c r="F126" s="14"/>
+      <c r="G126" s="14"/>
+      <c r="H126" s="14"/>
+      <c r="I126" s="14"/>
+      <c r="J126" s="6"/>
+      <c r="K126" s="15"/>
+    </row>
+    <row r="127" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A127" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="B126" s="114" t="s">
+      <c r="B127" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C126" s="115" t="s">
+      <c r="C127" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="D126" s="116"/>
-      <c r="E126" s="119" t="s">
+      <c r="D127" s="110"/>
+      <c r="E127" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="F126" s="120" t="s">
+      <c r="F127" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="G126" s="110" t="s">
+      <c r="G127" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="H126" s="112" t="s">
+      <c r="H127" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="I126" s="16"/>
-      <c r="J126" s="17"/>
-      <c r="K126" s="9"/>
-    </row>
-    <row r="127" spans="1:11">
-      <c r="A127" s="114"/>
-      <c r="B127" s="114"/>
-      <c r="C127" s="117"/>
-      <c r="D127" s="118"/>
-      <c r="E127" s="119"/>
-      <c r="F127" s="121"/>
-      <c r="G127" s="111"/>
-      <c r="H127" s="113"/>
-      <c r="I127" s="18"/>
-      <c r="J127" s="29"/>
-      <c r="K127" s="15"/>
+      <c r="I127" s="16"/>
+      <c r="J127" s="17"/>
+      <c r="K127" s="9"/>
     </row>
     <row r="128" spans="1:11">
-      <c r="A128" s="19">
+      <c r="A128" s="108"/>
+      <c r="B128" s="108"/>
+      <c r="C128" s="111"/>
+      <c r="D128" s="112"/>
+      <c r="E128" s="113"/>
+      <c r="F128" s="115"/>
+      <c r="G128" s="105"/>
+      <c r="H128" s="107"/>
+      <c r="I128" s="18"/>
+      <c r="J128" s="29"/>
+      <c r="K128" s="15"/>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="A129" s="19">
         <v>1</v>
       </c>
-      <c r="B128" s="70" t="s">
+      <c r="B129" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="C128" s="85" t="s">
+      <c r="C129" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="D128" s="88"/>
-      <c r="E128" s="82"/>
-      <c r="F128" s="68"/>
-      <c r="G128" s="91"/>
-      <c r="H128" s="20" t="s">
+      <c r="D129" s="88"/>
+      <c r="E129" s="82"/>
+      <c r="F129" s="68"/>
+      <c r="G129" s="91"/>
+      <c r="H129" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="I128" s="21"/>
-      <c r="J128" s="28"/>
-      <c r="K128" s="15"/>
-    </row>
-    <row r="129" spans="1:11" ht="84" customHeight="1">
-      <c r="A129" s="19">
-        <f>A128+1</f>
-        <v>2</v>
-      </c>
-      <c r="B129" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="C129" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="D129" s="101"/>
-      <c r="E129" s="102"/>
-      <c r="F129" s="103"/>
-      <c r="G129" s="100"/>
-      <c r="H129" s="107" t="s">
-        <v>79</v>
-      </c>
-      <c r="I129" s="108"/>
-      <c r="J129" s="109"/>
+      <c r="I129" s="21"/>
+      <c r="J129" s="28"/>
       <c r="K129" s="15"/>
     </row>
     <row r="130" spans="1:11">
       <c r="A130" s="19">
-        <f t="shared" ref="A130:A133" si="7">A129+1</f>
-        <v>3</v>
-      </c>
-      <c r="B130" s="71"/>
-      <c r="C130" s="86"/>
-      <c r="D130" s="88"/>
-      <c r="E130" s="88"/>
-      <c r="F130" s="68"/>
-      <c r="G130" s="91"/>
-      <c r="H130" s="93"/>
-      <c r="I130" s="21"/>
-      <c r="J130" s="22"/>
+        <f>A129+1</f>
+        <v>2</v>
+      </c>
+      <c r="B130" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="C130" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="D130" s="101"/>
+      <c r="E130" s="102"/>
+      <c r="F130" s="103"/>
+      <c r="G130" s="100"/>
+      <c r="H130" s="131" t="s">
+        <v>79</v>
+      </c>
+      <c r="I130" s="132"/>
+      <c r="J130" s="133"/>
       <c r="K130" s="15"/>
     </row>
     <row r="131" spans="1:11">
       <c r="A131" s="19">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="B131" s="72"/>
-      <c r="C131" s="87"/>
+        <f t="shared" ref="A131:A134" si="7">A130+1</f>
+        <v>3</v>
+      </c>
+      <c r="B131" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C131" s="85" t="s">
+        <v>75</v>
+      </c>
       <c r="D131" s="88"/>
       <c r="E131" s="82"/>
       <c r="F131" s="68"/>
       <c r="G131" s="91"/>
-      <c r="H131" s="93"/>
+      <c r="H131" s="93" t="s">
+        <v>84</v>
+      </c>
       <c r="I131" s="21"/>
       <c r="J131" s="22"/>
       <c r="K131" s="15"/>
@@ -3926,7 +4006,7 @@
     <row r="132" spans="1:11">
       <c r="A132" s="19">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B132" s="72"/>
       <c r="C132" s="87"/>
@@ -3942,64 +4022,268 @@
     <row r="133" spans="1:11">
       <c r="A133" s="19">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B133" s="72"/>
       <c r="C133" s="87"/>
-      <c r="D133" s="89"/>
-      <c r="E133" s="83"/>
-      <c r="F133" s="74"/>
-      <c r="G133" s="94"/>
-      <c r="H133" s="95"/>
-      <c r="I133" s="75"/>
-      <c r="J133" s="76"/>
+      <c r="D133" s="88"/>
+      <c r="E133" s="82"/>
+      <c r="F133" s="68"/>
+      <c r="G133" s="91"/>
+      <c r="H133" s="93"/>
+      <c r="I133" s="21"/>
+      <c r="J133" s="22"/>
       <c r="K133" s="15"/>
     </row>
     <row r="134" spans="1:11">
-      <c r="A134" s="23"/>
-      <c r="B134" s="24"/>
-      <c r="C134" s="25"/>
-      <c r="D134" s="90"/>
-      <c r="E134" s="84"/>
-      <c r="F134" s="69"/>
-      <c r="G134" s="97"/>
-      <c r="H134" s="98"/>
-      <c r="I134" s="26"/>
-      <c r="J134" s="27"/>
+      <c r="A134" s="19">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B134" s="72"/>
+      <c r="C134" s="87"/>
+      <c r="D134" s="89"/>
+      <c r="E134" s="83"/>
+      <c r="F134" s="74"/>
+      <c r="G134" s="94"/>
+      <c r="H134" s="95"/>
+      <c r="I134" s="75"/>
+      <c r="J134" s="76"/>
       <c r="K134" s="15"/>
     </row>
+    <row r="135" spans="1:11">
+      <c r="A135" s="23"/>
+      <c r="B135" s="24"/>
+      <c r="C135" s="25"/>
+      <c r="D135" s="90"/>
+      <c r="E135" s="84"/>
+      <c r="F135" s="69"/>
+      <c r="G135" s="97"/>
+      <c r="H135" s="98"/>
+      <c r="I135" s="26"/>
+      <c r="J135" s="27"/>
+      <c r="K135" s="15"/>
+    </row>
+    <row r="138" spans="1:11">
+      <c r="A138" s="13"/>
+      <c r="B138" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+      <c r="H138" s="13"/>
+    </row>
+    <row r="139" spans="1:11">
+      <c r="A139" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B139" s="14"/>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+      <c r="H139" s="14"/>
+      <c r="I139" s="14"/>
+      <c r="J139" s="6"/>
+      <c r="K139" s="15"/>
+    </row>
+    <row r="140" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A140" s="108" t="s">
+        <v>7</v>
+      </c>
+      <c r="B140" s="108" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140" s="109" t="s">
+        <v>4</v>
+      </c>
+      <c r="D140" s="110"/>
+      <c r="E140" s="113" t="s">
+        <v>6</v>
+      </c>
+      <c r="F140" s="114" t="s">
+        <v>47</v>
+      </c>
+      <c r="G140" s="104" t="s">
+        <v>39</v>
+      </c>
+      <c r="H140" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="I140" s="16"/>
+      <c r="J140" s="17"/>
+      <c r="K140" s="9"/>
+    </row>
+    <row r="141" spans="1:11">
+      <c r="A141" s="108"/>
+      <c r="B141" s="108"/>
+      <c r="C141" s="111"/>
+      <c r="D141" s="112"/>
+      <c r="E141" s="113"/>
+      <c r="F141" s="115"/>
+      <c r="G141" s="105"/>
+      <c r="H141" s="107"/>
+      <c r="I141" s="18"/>
+      <c r="J141" s="29"/>
+      <c r="K141" s="15"/>
+    </row>
+    <row r="142" spans="1:11">
+      <c r="A142" s="19">
+        <v>1</v>
+      </c>
+      <c r="B142" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="C142" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="D142" s="88"/>
+      <c r="E142" s="82"/>
+      <c r="F142" s="68"/>
+      <c r="G142" s="91"/>
+      <c r="H142" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="I142" s="21"/>
+      <c r="J142" s="28"/>
+      <c r="K142" s="15"/>
+    </row>
+    <row r="143" spans="1:11">
+      <c r="A143" s="19">
+        <f>A142+1</f>
+        <v>2</v>
+      </c>
+      <c r="B143" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C143" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="D143" s="101"/>
+      <c r="E143" s="102"/>
+      <c r="F143" s="103"/>
+      <c r="G143" s="100"/>
+      <c r="H143" s="131" t="s">
+        <v>84</v>
+      </c>
+      <c r="I143" s="132"/>
+      <c r="J143" s="133"/>
+      <c r="K143" s="15"/>
+    </row>
+    <row r="144" spans="1:11">
+      <c r="A144" s="19">
+        <f t="shared" ref="A144:A147" si="8">A143+1</f>
+        <v>3</v>
+      </c>
+      <c r="B144" s="70"/>
+      <c r="C144" s="85"/>
+      <c r="D144" s="88"/>
+      <c r="E144" s="82"/>
+      <c r="F144" s="68"/>
+      <c r="G144" s="91"/>
+      <c r="H144" s="93"/>
+      <c r="I144" s="21"/>
+      <c r="J144" s="22"/>
+      <c r="K144" s="15"/>
+    </row>
+    <row r="145" spans="1:11">
+      <c r="A145" s="19">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B145" s="72"/>
+      <c r="C145" s="87"/>
+      <c r="D145" s="88"/>
+      <c r="E145" s="82"/>
+      <c r="F145" s="68"/>
+      <c r="G145" s="91"/>
+      <c r="H145" s="93"/>
+      <c r="I145" s="21"/>
+      <c r="J145" s="22"/>
+      <c r="K145" s="15"/>
+    </row>
+    <row r="146" spans="1:11">
+      <c r="A146" s="19">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="B146" s="72"/>
+      <c r="C146" s="87"/>
+      <c r="D146" s="88"/>
+      <c r="E146" s="82"/>
+      <c r="F146" s="68"/>
+      <c r="G146" s="91"/>
+      <c r="H146" s="93"/>
+      <c r="I146" s="21"/>
+      <c r="J146" s="22"/>
+      <c r="K146" s="15"/>
+    </row>
+    <row r="147" spans="1:11">
+      <c r="A147" s="19">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="B147" s="72"/>
+      <c r="C147" s="87"/>
+      <c r="D147" s="89"/>
+      <c r="E147" s="83"/>
+      <c r="F147" s="74"/>
+      <c r="G147" s="94"/>
+      <c r="H147" s="95"/>
+      <c r="I147" s="75"/>
+      <c r="J147" s="76"/>
+      <c r="K147" s="15"/>
+    </row>
+    <row r="148" spans="1:11">
+      <c r="A148" s="23"/>
+      <c r="B148" s="24"/>
+      <c r="C148" s="25"/>
+      <c r="D148" s="90"/>
+      <c r="E148" s="84"/>
+      <c r="F148" s="69"/>
+      <c r="G148" s="97"/>
+      <c r="H148" s="98"/>
+      <c r="I148" s="26"/>
+      <c r="J148" s="27"/>
+      <c r="K148" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="H126:H127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="C126:D127"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:D91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="G90:G91"/>
-    <mergeCell ref="H90:H91"/>
-    <mergeCell ref="C44:D45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:H45"/>
-    <mergeCell ref="G57:H58"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
+  <mergeCells count="68">
+    <mergeCell ref="G140:G141"/>
+    <mergeCell ref="H140:H141"/>
+    <mergeCell ref="H143:J143"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="B140:B141"/>
+    <mergeCell ref="C140:D141"/>
+    <mergeCell ref="E140:E141"/>
+    <mergeCell ref="F140:F141"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="H130:J130"/>
+    <mergeCell ref="G103:G104"/>
+    <mergeCell ref="H103:H104"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="C115:D116"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="F115:F116"/>
+    <mergeCell ref="G115:G116"/>
+    <mergeCell ref="H115:H116"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="C103:D104"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="G24:H25"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
@@ -4007,29 +4291,36 @@
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="H129:J129"/>
-    <mergeCell ref="G102:G103"/>
-    <mergeCell ref="H102:H103"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="C114:D115"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="G114:G115"/>
-    <mergeCell ref="H114:H115"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="C102:D103"/>
-    <mergeCell ref="E102:E103"/>
-    <mergeCell ref="F102:F103"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="H91:H92"/>
+    <mergeCell ref="C45:D46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:H46"/>
+    <mergeCell ref="G58:H59"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="C78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="C91:D92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="G127:G128"/>
+    <mergeCell ref="H127:H128"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="B127:B128"/>
+    <mergeCell ref="C127:D128"/>
+    <mergeCell ref="E127:E128"/>
+    <mergeCell ref="F127:F128"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="3">
@@ -4039,7 +4330,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F128:G134 F92:G98 F79:G85 F104:G110 F116:G122 F26:F32" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F117:G123 F93:G99 F80:G86 F26:F33 F105:G111 F129:G135 F142:G148" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>